<commit_message>
excle data updated in commit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13530" windowHeight="4845" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
     <sheet name="FlipkartInput" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Title</t>
   </si>
@@ -151,16 +152,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>Him@nshu77990</t>
-  </si>
-  <si>
     <t>removeModel</t>
   </si>
   <si>
     <t>realme</t>
-  </si>
-  <si>
-    <t>8983844553</t>
   </si>
 </sst>
 </file>
@@ -758,7 +753,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -794,7 +789,7 @@
         <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -802,7 +797,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>38</v>
@@ -810,21 +805,14 @@
       <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="1" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>